<commit_message>
More Additions to testing script
</commit_message>
<xml_diff>
--- a/input/2021_pitcher_BR_link_database.xlsx
+++ b/input/2021_pitcher_BR_link_database.xlsx
@@ -186,9 +186,6 @@
     <t>Matt Shoemaker</t>
   </si>
   <si>
-    <t>Hyun Jin Ryu</t>
-  </si>
-  <si>
     <t>Nate Pearson</t>
   </si>
   <si>
@@ -369,9 +366,6 @@
     <t>Dakota Hudson</t>
   </si>
   <si>
-    <t>Matthew Boyd</t>
-  </si>
-  <si>
     <t>Tarik Skubal</t>
   </si>
   <si>
@@ -898,6 +892,12 @@
   </si>
   <si>
     <t>zeuchtj01</t>
+  </si>
+  <si>
+    <t>Matt Boyd</t>
+  </si>
+  <si>
+    <t>Hyun-Jin Ryu</t>
   </si>
 </sst>
 </file>
@@ -1297,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="F265" sqref="F265"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1310,7 +1310,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1393,7 +1393,7 @@
         <v>ma</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="3"/>
@@ -1420,7 +1420,7 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1464,7 +1464,7 @@
         <v>jo</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="3"/>
@@ -1800,7 +1800,7 @@
         <v>ca</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="3"/>
@@ -2112,7 +2112,7 @@
         <v>fr</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="3"/>
@@ -2184,7 +2184,7 @@
         <v>jo</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="3"/>
@@ -2328,7 +2328,7 @@
         <v>ch</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="3"/>
@@ -2481,15 +2481,15 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>292</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
-        <v>j</v>
+        <v>r</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
-        <v>jin r</v>
+        <v>ryu</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="2"/>
@@ -2499,12 +2499,12 @@
         <v>5</v>
       </c>
       <c r="F50" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
@@ -2528,7 +2528,7 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
@@ -2552,7 +2552,7 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
@@ -2600,7 +2600,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B56" t="str">
         <f t="shared" si="0"/>
@@ -2648,7 +2648,7 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="0"/>
@@ -2672,7 +2672,7 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="0"/>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="0"/>
@@ -2720,7 +2720,7 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="0"/>
@@ -2744,7 +2744,7 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61" t="str">
         <f t="shared" si="0"/>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B62" t="str">
         <f t="shared" si="0"/>
@@ -2792,7 +2792,7 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B63" t="str">
         <f t="shared" si="0"/>
@@ -2816,7 +2816,7 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B64" t="str">
         <f t="shared" si="0"/>
@@ -2840,7 +2840,7 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B65" t="str">
         <f t="shared" si="0"/>
@@ -2864,7 +2864,7 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B66" t="str">
         <f t="shared" si="0"/>
@@ -2888,7 +2888,7 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B67" t="str">
         <f t="shared" ref="B67:B130" si="4">LOWER(LEFT(MID(A67,FIND(" ",A67)+1,256),1))</f>
@@ -2903,7 +2903,7 @@
         <v>lu</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F67" t="str">
         <f t="shared" ref="F67:F130" si="7">C67&amp;D67&amp;E67</f>
@@ -2912,7 +2912,7 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B68" t="str">
         <f t="shared" si="4"/>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B69" t="str">
         <f t="shared" si="4"/>
@@ -2960,7 +2960,7 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B70" t="str">
         <f t="shared" si="4"/>
@@ -2978,12 +2978,12 @@
         <v>5</v>
       </c>
       <c r="F70" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B71" t="str">
         <f t="shared" si="4"/>
@@ -3007,7 +3007,7 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B72" t="str">
         <f t="shared" si="4"/>
@@ -3031,7 +3031,7 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73" t="str">
         <f t="shared" si="4"/>
@@ -3055,7 +3055,7 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B74" t="str">
         <f t="shared" si="4"/>
@@ -3079,7 +3079,7 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B75" t="str">
         <f t="shared" si="4"/>
@@ -3103,7 +3103,7 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B76" t="str">
         <f t="shared" si="4"/>
@@ -3127,7 +3127,7 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B77" t="str">
         <f t="shared" si="4"/>
@@ -3151,7 +3151,7 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B78" t="str">
         <f t="shared" si="4"/>
@@ -3175,7 +3175,7 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B79" t="str">
         <f t="shared" si="4"/>
@@ -3199,7 +3199,7 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B80" t="str">
         <f t="shared" si="4"/>
@@ -3214,7 +3214,7 @@
         <v>ma</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F80" t="str">
         <f t="shared" si="7"/>
@@ -3223,7 +3223,7 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B81" t="str">
         <f t="shared" si="4"/>
@@ -3247,7 +3247,7 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B82" t="str">
         <f t="shared" si="4"/>
@@ -3271,7 +3271,7 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B83" t="str">
         <f t="shared" si="4"/>
@@ -3295,7 +3295,7 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B84" t="str">
         <f t="shared" si="4"/>
@@ -3319,7 +3319,7 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B85" t="str">
         <f t="shared" si="4"/>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B86" t="str">
         <f t="shared" si="4"/>
@@ -3367,7 +3367,7 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B87" t="str">
         <f t="shared" si="4"/>
@@ -3391,7 +3391,7 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B88" t="str">
         <f t="shared" si="4"/>
@@ -3415,7 +3415,7 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B89" t="str">
         <f t="shared" si="4"/>
@@ -3439,7 +3439,7 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B90" t="str">
         <f t="shared" si="4"/>
@@ -3463,7 +3463,7 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B91" t="str">
         <f t="shared" si="4"/>
@@ -3487,7 +3487,7 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B92" t="str">
         <f t="shared" si="4"/>
@@ -3511,7 +3511,7 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B93" t="str">
         <f t="shared" si="4"/>
@@ -3535,7 +3535,7 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B94" t="str">
         <f t="shared" si="4"/>
@@ -3559,7 +3559,7 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B95" t="str">
         <f t="shared" si="4"/>
@@ -3583,7 +3583,7 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B96" t="str">
         <f t="shared" si="4"/>
@@ -3607,7 +3607,7 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B97" t="str">
         <f t="shared" si="4"/>
@@ -3622,7 +3622,7 @@
         <v>ro</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F97" t="str">
         <f t="shared" si="7"/>
@@ -3631,7 +3631,7 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B98" t="str">
         <f t="shared" si="4"/>
@@ -3655,7 +3655,7 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B99" t="str">
         <f t="shared" si="4"/>
@@ -3679,7 +3679,7 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B100" t="str">
         <f t="shared" si="4"/>
@@ -3703,7 +3703,7 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B101" t="str">
         <f t="shared" si="4"/>
@@ -3727,7 +3727,7 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B102" t="str">
         <f t="shared" si="4"/>
@@ -3751,7 +3751,7 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B103" t="str">
         <f t="shared" si="4"/>
@@ -3775,7 +3775,7 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B104" t="str">
         <f t="shared" si="4"/>
@@ -3799,7 +3799,7 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B105" t="str">
         <f t="shared" si="4"/>
@@ -3823,7 +3823,7 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B106" t="str">
         <f t="shared" si="4"/>
@@ -3847,7 +3847,7 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B107" t="str">
         <f t="shared" si="4"/>
@@ -3871,7 +3871,7 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B108" t="str">
         <f t="shared" si="4"/>
@@ -3895,7 +3895,7 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B109" t="str">
         <f t="shared" si="4"/>
@@ -3919,7 +3919,7 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B110" t="str">
         <f t="shared" si="4"/>
@@ -3943,7 +3943,7 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>116</v>
+        <v>291</v>
       </c>
       <c r="B111" t="str">
         <f t="shared" si="4"/>
@@ -3967,7 +3967,7 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B112" t="str">
         <f t="shared" si="4"/>
@@ -3991,7 +3991,7 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B113" t="str">
         <f t="shared" si="4"/>
@@ -4015,7 +4015,7 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B114" t="str">
         <f t="shared" si="4"/>
@@ -4039,7 +4039,7 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B115" t="str">
         <f t="shared" si="4"/>
@@ -4063,7 +4063,7 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B116" t="str">
         <f t="shared" si="4"/>
@@ -4087,7 +4087,7 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B117" t="str">
         <f t="shared" si="4"/>
@@ -4111,7 +4111,7 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B118" t="str">
         <f t="shared" si="4"/>
@@ -4135,7 +4135,7 @@
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B119" t="str">
         <f t="shared" si="4"/>
@@ -4159,7 +4159,7 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B120" t="str">
         <f t="shared" si="4"/>
@@ -4183,7 +4183,7 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B121" t="str">
         <f t="shared" si="4"/>
@@ -4207,7 +4207,7 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B122" t="str">
         <f t="shared" si="4"/>
@@ -4231,7 +4231,7 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B123" t="str">
         <f t="shared" si="4"/>
@@ -4255,7 +4255,7 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B124" t="str">
         <f t="shared" si="4"/>
@@ -4279,7 +4279,7 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B125" t="str">
         <f t="shared" si="4"/>
@@ -4303,7 +4303,7 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B126" t="str">
         <f t="shared" si="4"/>
@@ -4327,7 +4327,7 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B127" t="str">
         <f t="shared" si="4"/>
@@ -4351,7 +4351,7 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B128" t="str">
         <f t="shared" si="4"/>
@@ -4369,12 +4369,12 @@
         <v>5</v>
       </c>
       <c r="F128" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B129" t="str">
         <f t="shared" si="4"/>
@@ -4389,7 +4389,7 @@
         <v>br</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F129" t="str">
         <f t="shared" si="7"/>
@@ -4398,7 +4398,7 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B130" t="str">
         <f t="shared" si="4"/>
@@ -4422,7 +4422,7 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B131" t="str">
         <f t="shared" ref="B131:B193" si="8">LOWER(LEFT(MID(A131,FIND(" ",A131)+1,256),1))</f>
@@ -4446,7 +4446,7 @@
     </row>
     <row r="132" spans="1:6">
       <c r="A132" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B132" t="str">
         <f t="shared" si="8"/>
@@ -4470,7 +4470,7 @@
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B133" t="str">
         <f t="shared" si="8"/>
@@ -4494,7 +4494,7 @@
     </row>
     <row r="134" spans="1:6">
       <c r="A134" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B134" t="str">
         <f t="shared" si="8"/>
@@ -4518,7 +4518,7 @@
     </row>
     <row r="135" spans="1:6">
       <c r="A135" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B135" t="str">
         <f t="shared" si="8"/>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B136" t="str">
         <f t="shared" si="8"/>
@@ -4566,7 +4566,7 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B137" t="str">
         <f t="shared" si="8"/>
@@ -4590,7 +4590,7 @@
     </row>
     <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B138" t="str">
         <f t="shared" si="8"/>
@@ -4614,7 +4614,7 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B139" t="str">
         <f t="shared" si="8"/>
@@ -4638,7 +4638,7 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B140" t="str">
         <f t="shared" si="8"/>
@@ -4662,7 +4662,7 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B141" t="str">
         <f t="shared" si="8"/>
@@ -4686,7 +4686,7 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B142" t="str">
         <f t="shared" si="8"/>
@@ -4701,7 +4701,7 @@
         <v>al</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F142" t="str">
         <f t="shared" si="11"/>
@@ -4710,7 +4710,7 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B143" t="str">
         <f t="shared" si="8"/>
@@ -4734,7 +4734,7 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B144" t="str">
         <f t="shared" si="8"/>
@@ -4758,7 +4758,7 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B145" t="str">
         <f t="shared" si="8"/>
@@ -4782,7 +4782,7 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B146" t="str">
         <f t="shared" si="8"/>
@@ -4806,7 +4806,7 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B147" t="str">
         <f t="shared" si="8"/>
@@ -4824,12 +4824,12 @@
         <v>5</v>
       </c>
       <c r="F147" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B148" t="str">
         <f t="shared" si="8"/>
@@ -4853,7 +4853,7 @@
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B149" t="str">
         <f t="shared" si="8"/>
@@ -4877,7 +4877,7 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B150" t="str">
         <f t="shared" si="8"/>
@@ -4901,7 +4901,7 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B151" t="str">
         <f t="shared" si="8"/>
@@ -4925,7 +4925,7 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B152" t="str">
         <f t="shared" si="8"/>
@@ -4949,7 +4949,7 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B153" t="str">
         <f t="shared" si="8"/>
@@ -4973,7 +4973,7 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B154" t="str">
         <f t="shared" si="8"/>
@@ -4997,7 +4997,7 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B155" t="str">
         <f t="shared" si="8"/>
@@ -5021,7 +5021,7 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B156" t="str">
         <f t="shared" si="8"/>
@@ -5045,7 +5045,7 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B157" t="str">
         <f t="shared" si="8"/>
@@ -5060,7 +5060,7 @@
         <v>za</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F157" t="str">
         <f t="shared" si="11"/>
@@ -5069,7 +5069,7 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B158" t="str">
         <f t="shared" si="8"/>
@@ -5093,7 +5093,7 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B159" t="str">
         <f t="shared" si="8"/>
@@ -5117,7 +5117,7 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B160" t="str">
         <f t="shared" si="8"/>
@@ -5141,7 +5141,7 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B161" t="str">
         <f t="shared" si="8"/>
@@ -5165,7 +5165,7 @@
     </row>
     <row r="162" spans="1:6">
       <c r="A162" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B162" t="str">
         <f t="shared" si="8"/>
@@ -5189,7 +5189,7 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B163" t="str">
         <f t="shared" si="8"/>
@@ -5213,7 +5213,7 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B164" t="str">
         <f t="shared" si="8"/>
@@ -5237,7 +5237,7 @@
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B165" t="str">
         <f t="shared" si="8"/>
@@ -5261,7 +5261,7 @@
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B166" t="str">
         <f t="shared" si="8"/>
@@ -5285,7 +5285,7 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B167" t="str">
         <f t="shared" si="8"/>
@@ -5309,7 +5309,7 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B168" t="str">
         <f t="shared" si="8"/>
@@ -5324,7 +5324,7 @@
         <v>al</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F168" t="str">
         <f t="shared" si="11"/>
@@ -5333,7 +5333,7 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B169" t="str">
         <f t="shared" si="8"/>
@@ -5357,7 +5357,7 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B170" t="str">
         <f t="shared" si="8"/>
@@ -5381,7 +5381,7 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B171" t="str">
         <f t="shared" si="8"/>
@@ -5405,7 +5405,7 @@
     </row>
     <row r="172" spans="1:6">
       <c r="A172" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B172" t="str">
         <f t="shared" si="8"/>
@@ -5429,7 +5429,7 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B173" t="str">
         <f t="shared" si="8"/>
@@ -5453,7 +5453,7 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B174" t="str">
         <f t="shared" si="8"/>
@@ -5477,7 +5477,7 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B175" t="str">
         <f t="shared" si="8"/>
@@ -5501,7 +5501,7 @@
     </row>
     <row r="176" spans="1:6">
       <c r="A176" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B176" t="str">
         <f t="shared" si="8"/>
@@ -5525,7 +5525,7 @@
     </row>
     <row r="177" spans="1:6">
       <c r="A177" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B177" t="str">
         <f t="shared" si="8"/>
@@ -5540,7 +5540,7 @@
         <v>pa</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F177" t="str">
         <f t="shared" si="11"/>
@@ -5549,7 +5549,7 @@
     </row>
     <row r="178" spans="1:6">
       <c r="A178" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B178" t="str">
         <f t="shared" si="8"/>
@@ -5573,7 +5573,7 @@
     </row>
     <row r="179" spans="1:6">
       <c r="A179" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B179" t="str">
         <f t="shared" si="8"/>
@@ -5588,7 +5588,7 @@
         <v>jo</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F179" t="str">
         <f t="shared" si="11"/>
@@ -5597,7 +5597,7 @@
     </row>
     <row r="180" spans="1:6">
       <c r="A180" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B180" t="str">
         <f t="shared" si="8"/>
@@ -5621,7 +5621,7 @@
     </row>
     <row r="181" spans="1:6">
       <c r="A181" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B181" t="str">
         <f t="shared" si="8"/>
@@ -5645,7 +5645,7 @@
     </row>
     <row r="182" spans="1:6">
       <c r="A182" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B182" t="str">
         <f t="shared" si="8"/>
@@ -5669,7 +5669,7 @@
     </row>
     <row r="183" spans="1:6">
       <c r="A183" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B183" t="str">
         <f t="shared" si="8"/>
@@ -5693,7 +5693,7 @@
     </row>
     <row r="184" spans="1:6">
       <c r="A184" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B184" t="str">
         <f t="shared" si="8"/>
@@ -5708,7 +5708,7 @@
         <v>ca</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F184" t="str">
         <f t="shared" si="11"/>
@@ -5717,7 +5717,7 @@
     </row>
     <row r="185" spans="1:6">
       <c r="A185" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B185" t="str">
         <f t="shared" si="8"/>
@@ -5732,7 +5732,7 @@
         <v>jo</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F185" t="str">
         <f t="shared" si="11"/>
@@ -5741,7 +5741,7 @@
     </row>
     <row r="186" spans="1:6">
       <c r="A186" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B186" t="str">
         <f t="shared" si="8"/>
@@ -5765,7 +5765,7 @@
     </row>
     <row r="187" spans="1:6">
       <c r="A187" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B187" t="str">
         <f t="shared" si="8"/>
@@ -5789,7 +5789,7 @@
     </row>
     <row r="188" spans="1:6">
       <c r="A188" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B188" t="str">
         <f t="shared" si="8"/>
@@ -5804,7 +5804,7 @@
         <v>lu</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F188" t="str">
         <f t="shared" si="11"/>
@@ -5813,7 +5813,7 @@
     </row>
     <row r="189" spans="1:6">
       <c r="A189" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B189" t="str">
         <f t="shared" si="8"/>
@@ -5837,7 +5837,7 @@
     </row>
     <row r="190" spans="1:6">
       <c r="A190" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B190" t="str">
         <f t="shared" si="8"/>
@@ -5861,7 +5861,7 @@
     </row>
     <row r="191" spans="1:6">
       <c r="A191" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B191" t="str">
         <f t="shared" si="8"/>
@@ -5885,7 +5885,7 @@
     </row>
     <row r="192" spans="1:6">
       <c r="A192" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B192" t="str">
         <f t="shared" si="8"/>
@@ -5909,7 +5909,7 @@
     </row>
     <row r="193" spans="1:6">
       <c r="A193" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B193" t="str">
         <f t="shared" si="8"/>
@@ -5933,7 +5933,7 @@
     </row>
     <row r="194" spans="1:6">
       <c r="A194" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B194" t="str">
         <f t="shared" ref="B194:B257" si="12">LOWER(LEFT(MID(A194,FIND(" ",A194)+1,256),1))</f>
@@ -5957,7 +5957,7 @@
     </row>
     <row r="195" spans="1:6">
       <c r="A195" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B195" t="str">
         <f t="shared" si="12"/>
@@ -5981,7 +5981,7 @@
     </row>
     <row r="196" spans="1:6">
       <c r="A196" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B196" t="str">
         <f t="shared" si="12"/>
@@ -6005,7 +6005,7 @@
     </row>
     <row r="197" spans="1:6">
       <c r="A197" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B197" t="str">
         <f t="shared" si="12"/>
@@ -6029,7 +6029,7 @@
     </row>
     <row r="198" spans="1:6">
       <c r="A198" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B198" t="str">
         <f t="shared" si="12"/>
@@ -6053,7 +6053,7 @@
     </row>
     <row r="199" spans="1:6">
       <c r="A199" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B199" t="str">
         <f t="shared" si="12"/>
@@ -6077,7 +6077,7 @@
     </row>
     <row r="200" spans="1:6">
       <c r="A200" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B200" t="str">
         <f t="shared" si="12"/>
@@ -6101,7 +6101,7 @@
     </row>
     <row r="201" spans="1:6">
       <c r="A201" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B201" t="str">
         <f t="shared" si="12"/>
@@ -6125,7 +6125,7 @@
     </row>
     <row r="202" spans="1:6">
       <c r="A202" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B202" t="str">
         <f t="shared" si="12"/>
@@ -6149,7 +6149,7 @@
     </row>
     <row r="203" spans="1:6">
       <c r="A203" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B203" t="str">
         <f t="shared" si="12"/>
@@ -6173,7 +6173,7 @@
     </row>
     <row r="204" spans="1:6">
       <c r="A204" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B204" t="str">
         <f t="shared" si="12"/>
@@ -6197,7 +6197,7 @@
     </row>
     <row r="205" spans="1:6">
       <c r="A205" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B205" t="str">
         <f t="shared" si="12"/>
@@ -6221,7 +6221,7 @@
     </row>
     <row r="206" spans="1:6">
       <c r="A206" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B206" t="str">
         <f t="shared" si="12"/>
@@ -6245,7 +6245,7 @@
     </row>
     <row r="207" spans="1:6">
       <c r="A207" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B207" t="str">
         <f t="shared" si="12"/>
@@ -6269,7 +6269,7 @@
     </row>
     <row r="208" spans="1:6">
       <c r="A208" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B208" t="str">
         <f t="shared" si="12"/>
@@ -6284,7 +6284,7 @@
         <v>ry</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F208" t="str">
         <f t="shared" si="15"/>
@@ -6293,7 +6293,7 @@
     </row>
     <row r="209" spans="1:6">
       <c r="A209" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B209" t="str">
         <f t="shared" si="12"/>
@@ -6317,7 +6317,7 @@
     </row>
     <row r="210" spans="1:6">
       <c r="A210" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B210" t="str">
         <f t="shared" si="12"/>
@@ -6341,7 +6341,7 @@
     </row>
     <row r="211" spans="1:6">
       <c r="A211" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B211" t="str">
         <f t="shared" si="12"/>
@@ -6365,7 +6365,7 @@
     </row>
     <row r="212" spans="1:6">
       <c r="A212" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B212" t="str">
         <f t="shared" si="12"/>
@@ -6389,7 +6389,7 @@
     </row>
     <row r="213" spans="1:6">
       <c r="A213" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B213" t="str">
         <f t="shared" si="12"/>
@@ -6413,7 +6413,7 @@
     </row>
     <row r="214" spans="1:6">
       <c r="A214" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B214" t="str">
         <f t="shared" si="12"/>
@@ -6428,7 +6428,7 @@
         <v>jo</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F214" t="str">
         <f t="shared" si="15"/>
@@ -6437,7 +6437,7 @@
     </row>
     <row r="215" spans="1:6">
       <c r="A215" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B215" t="str">
         <f t="shared" si="12"/>
@@ -6461,7 +6461,7 @@
     </row>
     <row r="216" spans="1:6">
       <c r="A216" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B216" t="str">
         <f t="shared" si="12"/>
@@ -6509,7 +6509,7 @@
     </row>
     <row r="218" spans="1:6">
       <c r="A218" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B218" t="str">
         <f t="shared" si="12"/>
@@ -6533,7 +6533,7 @@
     </row>
     <row r="219" spans="1:6">
       <c r="A219" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B219" t="str">
         <f t="shared" si="12"/>
@@ -6557,7 +6557,7 @@
     </row>
     <row r="220" spans="1:6">
       <c r="A220" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B220" t="str">
         <f t="shared" si="12"/>
@@ -6581,7 +6581,7 @@
     </row>
     <row r="221" spans="1:6">
       <c r="A221" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B221" t="str">
         <f t="shared" si="12"/>
@@ -6599,12 +6599,12 @@
         <v>5</v>
       </c>
       <c r="F221" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="222" spans="1:6">
       <c r="A222" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B222" t="str">
         <f t="shared" si="12"/>
@@ -6628,7 +6628,7 @@
     </row>
     <row r="223" spans="1:6">
       <c r="A223" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B223" t="str">
         <f t="shared" si="12"/>
@@ -6652,7 +6652,7 @@
     </row>
     <row r="224" spans="1:6">
       <c r="A224" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B224" t="str">
         <f t="shared" si="12"/>
@@ -6676,7 +6676,7 @@
     </row>
     <row r="225" spans="1:6">
       <c r="A225" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B225" t="str">
         <f t="shared" si="12"/>
@@ -6700,7 +6700,7 @@
     </row>
     <row r="226" spans="1:6">
       <c r="A226" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B226" t="str">
         <f t="shared" si="12"/>
@@ -6724,7 +6724,7 @@
     </row>
     <row r="227" spans="1:6">
       <c r="A227" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B227" t="str">
         <f t="shared" si="12"/>
@@ -6742,12 +6742,12 @@
         <v>5</v>
       </c>
       <c r="F227" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="228" spans="1:6">
       <c r="A228" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B228" t="str">
         <f t="shared" si="12"/>
@@ -6771,7 +6771,7 @@
     </row>
     <row r="229" spans="1:6">
       <c r="A229" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B229" t="str">
         <f t="shared" si="12"/>
@@ -6795,7 +6795,7 @@
     </row>
     <row r="230" spans="1:6">
       <c r="A230" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B230" t="str">
         <f t="shared" si="12"/>
@@ -6819,7 +6819,7 @@
     </row>
     <row r="231" spans="1:6">
       <c r="A231" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B231" t="str">
         <f t="shared" si="12"/>
@@ -6843,7 +6843,7 @@
     </row>
     <row r="232" spans="1:6">
       <c r="A232" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B232" t="str">
         <f t="shared" si="12"/>
@@ -6867,7 +6867,7 @@
     </row>
     <row r="233" spans="1:6">
       <c r="A233" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B233" t="str">
         <f t="shared" si="12"/>
@@ -6891,7 +6891,7 @@
     </row>
     <row r="234" spans="1:6">
       <c r="A234" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B234" t="str">
         <f t="shared" si="12"/>
@@ -6915,7 +6915,7 @@
     </row>
     <row r="235" spans="1:6">
       <c r="A235" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B235" t="str">
         <f t="shared" si="12"/>
@@ -6939,7 +6939,7 @@
     </row>
     <row r="236" spans="1:6">
       <c r="A236" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B236" t="str">
         <f t="shared" si="12"/>
@@ -6963,7 +6963,7 @@
     </row>
     <row r="237" spans="1:6">
       <c r="A237" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B237" t="str">
         <f t="shared" si="12"/>
@@ -6987,7 +6987,7 @@
     </row>
     <row r="238" spans="1:6">
       <c r="A238" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B238" t="str">
         <f t="shared" si="12"/>
@@ -7011,7 +7011,7 @@
     </row>
     <row r="239" spans="1:6">
       <c r="A239" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B239" t="str">
         <f t="shared" si="12"/>
@@ -7035,7 +7035,7 @@
     </row>
     <row r="240" spans="1:6">
       <c r="A240" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B240" t="str">
         <f t="shared" si="12"/>
@@ -7059,7 +7059,7 @@
     </row>
     <row r="241" spans="1:6">
       <c r="A241" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B241" t="str">
         <f t="shared" si="12"/>
@@ -7083,7 +7083,7 @@
     </row>
     <row r="242" spans="1:6">
       <c r="A242" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B242" t="str">
         <f t="shared" si="12"/>
@@ -7101,12 +7101,12 @@
         <v>5</v>
       </c>
       <c r="F242" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="243" spans="1:6">
       <c r="A243" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B243" t="str">
         <f t="shared" si="12"/>
@@ -7130,7 +7130,7 @@
     </row>
     <row r="244" spans="1:6">
       <c r="A244" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B244" t="str">
         <f t="shared" si="12"/>
@@ -7154,7 +7154,7 @@
     </row>
     <row r="245" spans="1:6">
       <c r="A245" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B245" t="str">
         <f t="shared" si="12"/>
@@ -7178,7 +7178,7 @@
     </row>
     <row r="246" spans="1:6">
       <c r="A246" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B246" t="str">
         <f t="shared" si="12"/>
@@ -7202,7 +7202,7 @@
     </row>
     <row r="247" spans="1:6">
       <c r="A247" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B247" t="str">
         <f t="shared" si="12"/>
@@ -7217,7 +7217,7 @@
         <v>br</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F247" t="str">
         <f t="shared" si="15"/>
@@ -7226,7 +7226,7 @@
     </row>
     <row r="248" spans="1:6">
       <c r="A248" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B248" t="str">
         <f t="shared" si="12"/>
@@ -7250,7 +7250,7 @@
     </row>
     <row r="249" spans="1:6">
       <c r="A249" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B249" t="str">
         <f t="shared" si="12"/>
@@ -7268,12 +7268,12 @@
         <v>5</v>
       </c>
       <c r="F249" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="250" spans="1:6">
       <c r="A250" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B250" t="str">
         <f t="shared" si="12"/>
@@ -7297,7 +7297,7 @@
     </row>
     <row r="251" spans="1:6">
       <c r="A251" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B251" t="str">
         <f t="shared" si="12"/>
@@ -7312,7 +7312,7 @@
         <v>ma</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F251" t="str">
         <f t="shared" si="15"/>
@@ -7321,7 +7321,7 @@
     </row>
     <row r="252" spans="1:6">
       <c r="A252" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B252" t="str">
         <f t="shared" si="12"/>
@@ -7345,7 +7345,7 @@
     </row>
     <row r="253" spans="1:6">
       <c r="A253" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B253" t="str">
         <f t="shared" si="12"/>
@@ -7369,7 +7369,7 @@
     </row>
     <row r="254" spans="1:6">
       <c r="A254" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B254" t="str">
         <f t="shared" si="12"/>
@@ -7393,7 +7393,7 @@
     </row>
     <row r="255" spans="1:6">
       <c r="A255" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B255" t="str">
         <f t="shared" si="12"/>
@@ -7417,7 +7417,7 @@
     </row>
     <row r="256" spans="1:6">
       <c r="A256" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B256" t="str">
         <f t="shared" si="12"/>
@@ -7441,7 +7441,7 @@
     </row>
     <row r="257" spans="1:6">
       <c r="A257" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B257" t="str">
         <f t="shared" si="12"/>
@@ -7456,7 +7456,7 @@
         <v>ro</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F257" t="str">
         <f t="shared" si="15"/>
@@ -7465,7 +7465,7 @@
     </row>
     <row r="258" spans="1:6">
       <c r="A258" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B258" t="str">
         <f t="shared" ref="B258:B273" si="16">LOWER(LEFT(MID(A258,FIND(" ",A258)+1,256),1))</f>
@@ -7483,13 +7483,13 @@
         <v>5</v>
       </c>
       <c r="F258" t="str">
-        <f t="shared" ref="F258:F273" si="19">C258&amp;D258&amp;E258</f>
+        <f t="shared" ref="F258:F272" si="19">C258&amp;D258&amp;E258</f>
         <v>alexaty01</v>
       </c>
     </row>
     <row r="259" spans="1:6">
       <c r="A259" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B259" t="str">
         <f t="shared" si="16"/>
@@ -7513,7 +7513,7 @@
     </row>
     <row r="260" spans="1:6">
       <c r="A260" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B260" t="str">
         <f t="shared" si="16"/>
@@ -7528,7 +7528,7 @@
         <v>ca</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F260" t="str">
         <f t="shared" si="19"/>
@@ -7537,7 +7537,7 @@
     </row>
     <row r="261" spans="1:6">
       <c r="A261" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B261" t="str">
         <f t="shared" si="16"/>
@@ -7552,7 +7552,7 @@
         <v>jo</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F261" t="str">
         <f t="shared" si="19"/>
@@ -7561,7 +7561,7 @@
     </row>
     <row r="262" spans="1:6">
       <c r="A262" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B262" t="str">
         <f t="shared" si="16"/>
@@ -7576,7 +7576,7 @@
         <v>vi</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F262" t="str">
         <f t="shared" si="19"/>
@@ -7585,7 +7585,7 @@
     </row>
     <row r="263" spans="1:6">
       <c r="A263" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B263" t="str">
         <f t="shared" si="16"/>
@@ -7609,7 +7609,7 @@
     </row>
     <row r="264" spans="1:6">
       <c r="A264" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B264" t="str">
         <f t="shared" si="16"/>
@@ -7624,7 +7624,7 @@
         <v>ho</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F264" t="str">
         <f t="shared" si="19"/>
@@ -7633,7 +7633,7 @@
     </row>
     <row r="265" spans="1:6">
       <c r="A265" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B265" t="str">
         <f t="shared" si="16"/>
@@ -7657,7 +7657,7 @@
     </row>
     <row r="266" spans="1:6">
       <c r="A266" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B266" t="str">
         <f t="shared" si="16"/>
@@ -7681,7 +7681,7 @@
     </row>
     <row r="267" spans="1:6">
       <c r="A267" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B267" t="str">
         <f t="shared" si="16"/>
@@ -7705,7 +7705,7 @@
     </row>
     <row r="268" spans="1:6">
       <c r="A268" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B268" t="str">
         <f t="shared" si="16"/>
@@ -7729,7 +7729,7 @@
     </row>
     <row r="269" spans="1:6">
       <c r="A269" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B269" t="str">
         <f t="shared" si="16"/>
@@ -7753,7 +7753,7 @@
     </row>
     <row r="270" spans="1:6">
       <c r="A270" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B270" t="str">
         <f t="shared" si="16"/>
@@ -7777,7 +7777,7 @@
     </row>
     <row r="271" spans="1:6">
       <c r="A271" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B271" t="str">
         <f t="shared" si="16"/>
@@ -7801,7 +7801,7 @@
     </row>
     <row r="272" spans="1:6">
       <c r="A272" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B272" t="str">
         <f t="shared" si="16"/>
@@ -7825,7 +7825,7 @@
     </row>
     <row r="273" spans="1:6">
       <c r="A273" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B273" t="str">
         <f t="shared" si="16"/>
@@ -7843,7 +7843,7 @@
         <v>5</v>
       </c>
       <c r="F273" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>